<commit_message>
Add function of removing new lines which has no meaning
</commit_message>
<xml_diff>
--- a/Ax2/parser_table.xlsx
+++ b/Ax2/parser_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e013e576aa07c75d/Documents/GitHub/Flowcode/Ax2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_F25DC773A252ABDACC104864D99F446E5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C85CD32A-9F34-4CF9-A1B7-0C80FF4006F8}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="11_F25DC773A252ABDACC104864D99F446E5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594C3E21-F0D0-431F-A078-69A9F5C528C2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>FIRST</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Identifier</t>
   </si>
   <si>
-    <t>Identifier, Input, Output, Return, ε</t>
-  </si>
-  <si>
     <t>Comma, ε</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>SemiColon</t>
   </si>
   <si>
-    <t>EndOfLine</t>
-  </si>
-  <si>
     <t>Int, Double, String, Boolean, ε</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Comma, RightParen</t>
   </si>
   <si>
-    <t>Identifier, Input, Output, Return, End</t>
-  </si>
-  <si>
     <t>EndOfLine, RightParen</t>
   </si>
   <si>
@@ -174,16 +165,94 @@
     <t>EndOfLine, SemiColon</t>
   </si>
   <si>
-    <t>Int, Double, String, Boolean, EndOfLine</t>
-  </si>
-  <si>
     <t>&lt;program&gt; -&gt; Begin Colon EndOfLine &lt;declaration_section&gt; &lt;function_definition&gt; End SemiColon | ε</t>
   </si>
   <si>
-    <t>&lt;statement&gt; -&gt; &lt;assignment_statement&gt; | &lt;input_statement&gt; | &lt;output_statement&gt; | &lt;return_statement&gt; | ε</t>
-  </si>
-  <si>
-    <t>&lt;statement_list&gt; -&gt; &lt;statement&gt; &lt;statement_list&gt;</t>
+    <t>&lt;repeat_statement&gt; -&gt; Check &lt;condition&gt; Colon EndOfLine &lt;repeat_statement_list&gt; Repeat SemiColon EndOfLine</t>
+  </si>
+  <si>
+    <t>&lt;repeat_statement_list&gt; -&gt; &lt;repeat_statement_line&gt; &lt;repeat_statement_list&gt; | ε</t>
+  </si>
+  <si>
+    <t>&lt;repeat_statement_line&gt; -&gt; &lt;assignment_statement&gt; | &lt;input_statement&gt; | &lt;output_statement&gt; | &lt;return_statement&gt; | &lt;repeat_statement&gt; | Break EndOfLine | Continue EndOfLine</t>
+  </si>
+  <si>
+    <t>&lt;condition&gt; -&gt; &lt;bool_term&gt; &lt;bool_expr_tail&gt;</t>
+  </si>
+  <si>
+    <t>&lt;bool_expr_tail&gt; -&gt; LogicalAnd &lt;bool_term&gt; &lt;bool_expr_tail&gt; | LogicalOr &lt;bool_term&gt; &lt;bool_expr_tail&gt; | ε</t>
+  </si>
+  <si>
+    <t>&lt;bool_term&gt; -&gt; LogicalNot &lt;basic_bool&gt; | &lt;basic_bool&gt;</t>
+  </si>
+  <si>
+    <t>&lt;basic_bool&gt; -&gt; True | False | &lt;operand&gt; &lt;compare_op&gt; &lt;operand&gt; | LeftParen &lt;bool_expr&gt; RightParen</t>
+  </si>
+  <si>
+    <t>&lt;operand&gt; -&gt; Identifier | IntLiteral | DoubleLiteral | StringLiteral | True | False</t>
+  </si>
+  <si>
+    <t>&lt;compare_op&gt; -&gt; Equal | NotEqual | LessThan | GreaterThan | LessOrEqual | GreaterOrEqual</t>
+  </si>
+  <si>
+    <t>Identifier, IntLiteral, DoubleLiteral, StringLiteral, True, False</t>
+  </si>
+  <si>
+    <t>Equal, NotEqual, LessThan, GreaterThan, LessOrEqual, GreaterOrEqual</t>
+  </si>
+  <si>
+    <t>True, False, Identifier, IntLiteral, DoubleLiteral, StringLiteral, LeftParen</t>
+  </si>
+  <si>
+    <t>LogicalNot, True, False, Identifier, IntLiteral, DoubleLiteral, StringLiteral, LeftParen</t>
+  </si>
+  <si>
+    <t>LogicalAnd, LogicalOr, ε</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, Break, Continue, ε</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, Break, Continue</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>&lt;statement&gt; -&gt; &lt;assignment_statement&gt; | &lt;input_statement&gt; | &lt;output_statement&gt; | &lt;return_statement&gt; | &lt;repeat_statement&gt;</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check</t>
+  </si>
+  <si>
+    <t>&lt;statement_list&gt; -&gt; &lt;statement&gt; &lt;statement_list&gt; | ε</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, ε</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, End</t>
+  </si>
+  <si>
+    <t>Multiply, Divide, Modulo, Add, Subtract, EndOfLine, RightParen, Power</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, Break, Continue, End</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Identifier, Input, Output, Return, Check, Break, Continue, Repeat</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>LogicalAnd, LogicalOr, Colon</t>
+  </si>
+  <si>
+    <t>Equal, NotEqual, LessThan, GreaterThan, LessOrEqual, GreaterOrEqual, LogicalAnd, LogicalOr, Colon</t>
   </si>
 </sst>
 </file>
@@ -272,6 +341,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,16 +610,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="129.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="56" style="1" customWidth="1"/>
+    <col min="1" max="1" width="157.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="57.85546875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -562,13 +635,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
@@ -584,13 +657,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,10 +682,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +696,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,21 +704,21 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,10 +726,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,10 +737,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,32 +748,32 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +784,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +795,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +806,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -755,7 +828,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,7 +839,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,29 +850,29 @@
         <v>23</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +894,106 @@
         <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete function(main, custom), repeat, special keyword(return, break, continue,..), declaration, assignment, complex operation, whole program structure
</commit_message>
<xml_diff>
--- a/Ax2/parser_table.xlsx
+++ b/Ax2/parser_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e013e576aa07c75d/Documents/GitHub/Flowcode/Ax2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="11_F25DC773A252ABDACC104864D99F446E5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C88B7D97-E6DB-4B5E-B35A-15B9AC72E627}"/>
+  <xr:revisionPtr revIDLastSave="411" documentId="11_F25DC773A252ABDACC104864D99F446E5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44A83CEC-6AC9-44AD-845D-D37F04F30AF9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>FIRST</t>
   </si>
@@ -294,13 +294,10 @@
     <t>Equal, NotEqual, LessThan, GreaterThan, LessOrEqual, GreaterOrEqual, LogicalAnd, LogicalOr, Colon, RightParen</t>
   </si>
   <si>
-    <t>Add, Subtract, EndOfLine, RightParen, RightParen, Comma, SemiColon</t>
-  </si>
-  <si>
     <t>Power, Multiply, Divide, Modulo, Add, Subtract, EndOfLine, RightParen, Comma, SemiColon</t>
   </si>
   <si>
-    <t>&lt;factor&gt; -&gt; IntLiteral | StringLiteral | DoubleLiteral | LeftParen &lt;expression&gt; RightParen | Identifier | Identifier Colon &lt;argument_list&gt;</t>
+    <t>&lt;factor&gt; -&gt; IntLiteral | StringLiteral | DoubleLiteral | LeftParen &lt;expression&gt; RightParen | Identifier | Identifier Colon &lt;argument_list&gt; SemiColon</t>
   </si>
 </sst>
 </file>
@@ -386,10 +383,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,16 +650,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="97" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="174.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="102.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -922,13 +916,13 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,7 +1109,7 @@
         <v>21</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1131,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>